<commit_message>
updates done upto 17Jan2023
</commit_message>
<xml_diff>
--- a/HybridFramework_635Batch/src/test/resources/testdata/TD.xlsx
+++ b/HybridFramework_635Batch/src/test/resources/testdata/TD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nalla\git\repository635HFW\HybridFramework_635Batch\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90B80A4-4C08-49FA-867B-510CAA8FE944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2AEEBC-9A41-4A04-A81C-7986D31CB373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Zeba</t>
   </si>
@@ -112,12 +112,6 @@
     <t>h56745tgngfhfg</t>
   </si>
   <si>
-    <t>er6453</t>
-  </si>
-  <si>
-    <t>tryt76575</t>
-  </si>
-  <si>
     <t>gu5674</t>
   </si>
   <si>
@@ -128,6 +122,12 @@
   </si>
   <si>
     <t>cvbncvnvcnvsdg</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -654,10 +654,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF52FC43-BD58-49AE-BFE4-55FD751288D5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,7 +684,9 @@
       <c r="B2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
@@ -693,43 +695,42 @@
       <c r="B3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -763,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A47E26-B505-4FE7-9528-B913AF9A7EB7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,6 +792,9 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -799,6 +803,9 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -807,6 +814,9 @@
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -815,6 +825,9 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -823,6 +836,9 @@
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -831,6 +847,9 @@
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -838,6 +857,9 @@
       </c>
       <c r="B8" t="s">
         <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>